<commit_message>
-- Scale Document Understanding App fully functional
</commit_message>
<xml_diff>
--- a/sample_data/out/Report.xlsx
+++ b/sample_data/out/Report.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black-XL-ROSE\Documents\UiPath\Invoice_Document_Understanding\sample_data\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B99EDF4-DA12-4245-B85A-153BD592E289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECE33D-DAEE-4E89-A158-357F34802B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="1845" windowWidth="18000" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="345" yWindow="660" windowWidth="18000" windowHeight="11655" xr2:uid="{54939239-8781-4574-B03B-2B0788971A68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Invoice Number</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>INV-10012</t>
+  </si>
+  <si>
+    <t>A246</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -124,7 +127,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -171,6 +174,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -206,6 +226,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -357,20 +394,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D33764-B718-48A0-9AE6-11BBB27FCB5A}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -398,6 +427,48 @@
       </c>
       <c r="D2">
         <v>1699.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44281</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44311</v>
+      </c>
+      <c r="D3">
+        <v>1699.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>202205</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44712</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44726</v>
+      </c>
+      <c r="D4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43174</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43205</v>
+      </c>
+      <c r="D5">
+        <v>700.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-- Use Generative Extraction
</commit_message>
<xml_diff>
--- a/sample_data/out/Report.xlsx
+++ b/sample_data/out/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black-XL-ROSE\Documents\UiPath\Invoice_Document_Understanding\sample_data\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B99EDF4-DA12-4245-B85A-153BD592E289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A044C4-14A0-45F7-9620-A353E57A6119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="1845" windowWidth="18000" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="3720" windowWidth="14430" windowHeight="7725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Invoice Number</t>
   </si>
@@ -36,16 +36,42 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>INV-10012</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
+  </si>
+  <si>
+    <t>Line Items</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Payment Terms</t>
+  </si>
+  <si>
+    <t>26/3/2021</t>
+  </si>
+  <si>
+    <t>25/4/2021</t>
+  </si>
+  <si>
+    <t>- Services, $55.00, 10, $550.00
+- Consulting, $75.00, 15, $1,125.00
+- Materials, $123.39, 1, $123.39</t>
+  </si>
+  <si>
+    <t>Please pay within 30 days using the link in your invoice email.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R&quot;#,##0.00_);[Red]\(&quot;R&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,9 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,7 +388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -372,7 +402,7 @@
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,21 +413,36 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44281</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44311</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3">
         <v>1699.48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>